<commit_message>
Added literature notes for Mancinelli et al 2002
Edited the EtOH ms for PRISM
</commit_message>
<xml_diff>
--- a/lab_docs/manuscripts/LitSurvey.xlsx
+++ b/lab_docs/manuscripts/LitSurvey.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>Bugs</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Pond</t>
   </si>
   <si>
-    <t>Szkokan_Emilson 2011</t>
-  </si>
-  <si>
     <t>Pabst and Scheifhacken 2008</t>
   </si>
   <si>
@@ -82,13 +79,85 @@
   </si>
   <si>
     <t>Mancinelli and Costantini</t>
+  </si>
+  <si>
+    <t>Szkokan and Emilson 2011</t>
+  </si>
+  <si>
+    <t>Bohmann and Hermann 2006</t>
+  </si>
+  <si>
+    <t>Brady and Turner 2012</t>
+  </si>
+  <si>
+    <t>mesocosm</t>
+  </si>
+  <si>
+    <t>Freschet et al. 2012</t>
+  </si>
+  <si>
+    <t>frozen</t>
+  </si>
+  <si>
+    <t>Bottollier et al. 2011</t>
+  </si>
+  <si>
+    <t>Brainard and Fairchild 2012</t>
+  </si>
+  <si>
+    <t>cores</t>
+  </si>
+  <si>
+    <t>Francis et al. 2007</t>
+  </si>
+  <si>
+    <t>litter bags and Ekmans</t>
+  </si>
+  <si>
+    <t>Hansen et al. 1998</t>
+  </si>
+  <si>
+    <t>core incubations</t>
+  </si>
+  <si>
+    <t>OM subsampled</t>
+  </si>
+  <si>
+    <t>sep. samples</t>
+  </si>
+  <si>
+    <t>Pope et al. 1999</t>
+  </si>
+  <si>
+    <t>litter mesocosms</t>
+  </si>
+  <si>
+    <t>Stenert et al. 2012</t>
+  </si>
+  <si>
+    <t>undesc. Sed sample</t>
+  </si>
+  <si>
+    <t>sep. sweep nets</t>
+  </si>
+  <si>
+    <t>Stewart and Downing 2008</t>
+  </si>
+  <si>
+    <t>formalin -&gt; ethanol</t>
+  </si>
+  <si>
+    <t>stovepipe sample</t>
+  </si>
+  <si>
+    <t>Li and Dudheon 2008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +173,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -121,13 +203,178 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,161 +669,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="15.75">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" ht="15.75">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75">
+      <c r="A15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75">
+      <c r="A16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
+      <c r="A19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>